<commit_message>
Model Traning Code Source
model_traning: onde o modelo NLP treina e testa o modelo
MailboxTraining.py: leitura advinda da mailbox
Config_TreinoModelo.xlsx: Config do modelo
</commit_message>
<xml_diff>
--- a/Config_TreinoModelo.xlsx
+++ b/Config_TreinoModelo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://groupecgi-my.sharepoint.com/personal/brunofilipe_lobo_cgi_com/Documents/Code/realvidaseguros/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nayara.rodrigues\Documents\RVS-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC1048DA19DC7D545ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A68EA4D-6A0A-4F99-9CBB-3FFBF0322F56}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65485F0-126F-40D6-9731-3A3314418CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,48 +36,9 @@
     <t>desc</t>
   </si>
   <si>
-    <t>EmailGIO</t>
-  </si>
-  <si>
-    <t>RVS.CGI2@realvidaseguros.onmicrosoft.com</t>
-  </si>
-  <si>
-    <t>Email Acesso GIO</t>
-  </si>
-  <si>
-    <t>PasswordGIO</t>
-  </si>
-  <si>
-    <t>Piriquit0!</t>
-  </si>
-  <si>
-    <t>Password Acesso GIO</t>
-  </si>
-  <si>
-    <t>LinkGIO</t>
-  </si>
-  <si>
-    <t>https://webcrm_qld.realvidaseguros.pt/</t>
-  </si>
-  <si>
-    <t>Link GIO QLD</t>
-  </si>
-  <si>
-    <t>PathDriverEdge</t>
-  </si>
-  <si>
-    <t>realvidaseguros\lib\msedgedriver.exe</t>
-  </si>
-  <si>
-    <t>Path do Driver do Edge</t>
-  </si>
-  <si>
     <t>SQLExpressServer</t>
   </si>
   <si>
-    <t>PT-L164962\SQLEXPRESS</t>
-  </si>
-  <si>
     <t>Servidor SQL Express</t>
   </si>
   <si>
@@ -90,63 +51,21 @@
     <t>Database a conectar</t>
   </si>
   <si>
-    <t>TableName</t>
-  </si>
-  <si>
-    <t>Emails_IPA_NLP</t>
-  </si>
-  <si>
-    <t>Nome da tabela</t>
-  </si>
-  <si>
     <t>MailboxName</t>
   </si>
   <si>
-    <t>brunofilipe.lobo@cgi.com</t>
-  </si>
-  <si>
     <t>Nome da Mailbox a Usar (email)</t>
   </si>
   <si>
     <t>InboxFolder</t>
   </si>
   <si>
-    <t>RVS</t>
-  </si>
-  <si>
     <t>Nome da pasta a ir buscar emails</t>
   </si>
   <si>
-    <t>EmailsToMove</t>
-  </si>
-  <si>
-    <t>RVS_Em Tratamento</t>
-  </si>
-  <si>
-    <t>Nome da pasta a mover os emails depois de lidos</t>
-  </si>
-  <si>
-    <t>SenderEmailException</t>
-  </si>
-  <si>
-    <t>"Real Vida Seguros" &lt;noreply@realvidaseguros.pt&gt;|Real Vida Seguros &lt;noreply@realvidaseguros.pt&gt;|"RV - Formulário Contactos" &lt;noreply@realvidaseguros.pt&gt;|RV - Formulário Contactos &lt;noreply2@realvidaseguros.pt&gt;|"Real Vida Seguros" &lt;gisdoc@realvidaseguros.pt&gt;</t>
-  </si>
-  <si>
-    <t>QueueTableName</t>
-  </si>
-  <si>
-    <t>QueueItem</t>
-  </si>
-  <si>
-    <t>Nome tabela Queue</t>
-  </si>
-  <si>
     <t>LogsTableName</t>
   </si>
   <si>
-    <t>LOGS</t>
-  </si>
-  <si>
     <t>Nome tabela Logs</t>
   </si>
   <si>
@@ -168,19 +87,100 @@
     <t>Caminho da classificacao de apolices</t>
   </si>
   <si>
-    <t>TrustScore</t>
-  </si>
-  <si>
-    <t>Score Confiado para Tratamento</t>
-  </si>
-  <si>
     <t>Emails de excepcao onde o dispatcher extrai automaticamente o NIF e Nome do Cliente</t>
   </si>
   <si>
-    <t>realvidaseguros\IntelligentProcessAutomationNLP\Automation\classificacaoapolices.xlsx</t>
-  </si>
-  <si>
-    <t>realvidaseguros\IntelligentProcessAutomationNLP\Automation\intencoes.xlsx</t>
+    <t>NomeProcesso</t>
+  </si>
+  <si>
+    <t>Adefinir</t>
+  </si>
+  <si>
+    <t>Nome do Processo (a aparecer nos logs)</t>
+  </si>
+  <si>
+    <t>PT-L163255\SQLEXPRESS01</t>
+  </si>
+  <si>
+    <t>nayara.rodrigues@cgi.com</t>
+  </si>
+  <si>
+    <t>SenderEmailExtract</t>
+  </si>
+  <si>
+    <t>"Real Vida Seguros" &lt;noreply@realvidaseguros.pt&gt;|Real Vida Seguros &lt;noreply@realvidaseguros.pt&gt;|"RV - Formulário Contactos" &lt;noreply@realvidaseguros.pt&gt;|RV - Formulário Contactos &lt;noreply2@realvidaseguros.pt&gt;|"Real Vida Seguros" &lt;gisdoc@realvidaseguros.pt&gt;|Real Vida Seguros &lt;gisdoc@realvidaseguros.pt&gt;</t>
+  </si>
+  <si>
+    <t>SenderEmailDiscard</t>
+  </si>
+  <si>
+    <t>Real Vida Seguros &lt;noreply2@realvidaseguros.pt&gt;|Clientes Real Vida &lt;info.clientes@realvidaseguros.pt&gt;</t>
+  </si>
+  <si>
+    <t>Emails de excepcao onde o dispatcher discarta automaticamente o email</t>
+  </si>
+  <si>
+    <t>IntelligentProcessAutomationNLP\Automation\intencoes.xlsx</t>
+  </si>
+  <si>
+    <t>IntelligentProcessAutomationNLP\Automation\classificacaoapolices.xlsx</t>
+  </si>
+  <si>
+    <t>Base_Dir</t>
+  </si>
+  <si>
+    <t>IntelligentProcessAutomationNLP/ModelNLP/</t>
+  </si>
+  <si>
+    <t>Diretorio Base do Projeto</t>
+  </si>
+  <si>
+    <t>TokenizerPath</t>
+  </si>
+  <si>
+    <t>tokenizer</t>
+  </si>
+  <si>
+    <t>Diretorio do Tokenizer (Convem estar dentro do diretorio base do projeto)</t>
+  </si>
+  <si>
+    <t>Model_Path</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>Diretorio do Modelo NLP (Convem estar dentro do diretorio base do projeto)</t>
+  </si>
+  <si>
+    <t>NumLabelsNLP</t>
+  </si>
+  <si>
+    <t>Numero Labels Modelo NLP</t>
+  </si>
+  <si>
+    <t>SheetRegrasPreTratamento</t>
+  </si>
+  <si>
+    <t>RegrasEmailsPreTratamento</t>
+  </si>
+  <si>
+    <t>SheetRegrasEmailDiscard</t>
+  </si>
+  <si>
+    <t>RegrasEmailDiscard</t>
+  </si>
+  <si>
+    <t>PathConfigRegrasEmails</t>
+  </si>
+  <si>
+    <t>IntelligentProcessAutomationNLP\Automation\RegrasEmails.xlsx</t>
+  </si>
+  <si>
+    <t>LOGS_TREINO</t>
+  </si>
+  <si>
+    <t>Modelo de Dados NLP</t>
   </si>
 </sst>
 </file>
@@ -498,20 +498,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="248.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="133.88671875" customWidth="1"/>
+    <col min="3" max="3" width="83.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -522,197 +522,202 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
       </c>
       <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18">
-        <v>0.1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;8&amp;K000000  &amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{f5b21038-f9e1-4e7d-8ce4-653ce59968ea}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" removed="0"/>
+  <clbl:label id="{f5b21038-f9e1-4e7d-8ce4-653ce59968ea}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>